<commit_message>
find summary function working
</commit_message>
<xml_diff>
--- a/Test.xlsx
+++ b/Test.xlsx
@@ -6,8 +6,8 @@
     <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Data" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="FAQ" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="FAQ" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Data" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="Weekly Summary" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
@@ -1199,6 +1199,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:1"/>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -4191,27 +4212,6 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:1"/>
-  </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>

</xml_diff>